<commit_message>
Even more work on rugged tablet project.
</commit_message>
<xml_diff>
--- a/docs/_projects/rugged-tablet-parts.xlsx
+++ b/docs/_projects/rugged-tablet-parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\zofware\www.simplesportscaster.com\docs\_projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD73DA7-C2DC-4B76-9877-DBDD8BDBD972}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65034F8F-6E08-4100-8566-633251CFD75C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10380" yWindow="1390" windowWidth="24030" windowHeight="18430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13850" yWindow="1640" windowWidth="24030" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
   <si>
     <t>Manfrotto 2909+2907</t>
   </si>
@@ -257,12 +257,37 @@
   <si>
     <t>screws, nuts, solder, wires, drill, bits, screwdriver, soldering iron, wire cutter</t>
   </si>
+  <si>
+    <t>right angle 3.5mm headphone extension 3ft</t>
+  </si>
+  <si>
+    <t>Stays plugged into tablet to receive audio feed from pole mounted microphone</t>
+  </si>
+  <si>
+    <t>YCS Basics</t>
+  </si>
+  <si>
+    <t>3.5mm headphone extension 25 ft</t>
+  </si>
+  <si>
+    <t>Brings microphone feed down the camera pole</t>
+  </si>
+  <si>
+    <t>PowerDeWise</t>
+  </si>
+  <si>
+    <t>Omnidirectional label microphone</t>
+  </si>
+  <si>
+    <t>Mount next to Sony HDR-CX405 camera to provide audio feed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -320,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -331,12 +356,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="35">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -615,68 +655,85 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4C557803-1D46-4E4C-A4C3-4D68A9649F0C}" name="Table13" displayName="Table13" ref="A2:F16" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4C557803-1D46-4E4C-A4C3-4D68A9649F0C}" name="Table13" displayName="Table13" ref="A2:F16" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="A2:F16" xr:uid="{A1543D44-F302-4351-9E6B-4276A16DF2F1}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{EA0DB7B1-C470-46D6-9C12-3FFDAC9B51D9}" name="Manufacturer" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{69307F5A-31AB-4FBD-8507-A82313D79606}" name="Part" dataDxfId="28" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{9A448ED8-5613-4F22-83B1-5C6087672567}" name="Quantity" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{37A5C064-2E7B-45AC-A7D3-1D0079B2F80B}" name="Unit Cost" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{72C5C51A-2F4A-4C3E-A858-3899C33EB849}" name="Total Cost" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{EA0DB7B1-C470-46D6-9C12-3FFDAC9B51D9}" name="Manufacturer" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{69307F5A-31AB-4FBD-8507-A82313D79606}" name="Part" dataDxfId="31" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{9A448ED8-5613-4F22-83B1-5C6087672567}" name="Quantity" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{37A5C064-2E7B-45AC-A7D3-1D0079B2F80B}" name="Unit Cost" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{72C5C51A-2F4A-4C3E-A858-3899C33EB849}" name="Total Cost" dataDxfId="28">
       <calculatedColumnFormula>C3*D3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8C774BF9-72A7-40C2-848A-EC6B719C339F}" name="Description" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{8C774BF9-72A7-40C2-848A-EC6B719C339F}" name="Description" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{67FCDD6A-3F4B-4E9E-A876-51C576C314B4}" name="Table14" displayName="Table14" ref="A18:F22" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{67FCDD6A-3F4B-4E9E-A876-51C576C314B4}" name="Table14" displayName="Table14" ref="A18:F22" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A18:F22" xr:uid="{707D3113-7CC3-418A-92EC-DDA3DF334183}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BC3C2856-73B8-4559-AA00-E102B3063D2E}" name="Manufacturer" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{1CF2A33E-5769-4A72-93D7-538F4D4752E0}" name="Part" dataDxfId="20" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{499A5FED-4581-4C92-8F7E-BA159D69E568}" name="Quantity" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{4AF0BC0F-C86A-41A2-B354-5CD8BB6738E2}" name="Unit Cost" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{5642BBD2-4BF5-4B35-B008-F3DAACFCBBC0}" name="Total Cost" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{BC3C2856-73B8-4559-AA00-E102B3063D2E}" name="Manufacturer" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{1CF2A33E-5769-4A72-93D7-538F4D4752E0}" name="Part" dataDxfId="23" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{499A5FED-4581-4C92-8F7E-BA159D69E568}" name="Quantity" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{4AF0BC0F-C86A-41A2-B354-5CD8BB6738E2}" name="Unit Cost" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{5642BBD2-4BF5-4B35-B008-F3DAACFCBBC0}" name="Total Cost" dataDxfId="20">
       <calculatedColumnFormula>C19*D19</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{03D6D45C-954A-4270-8DD8-B4A135956956}" name="Description" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{03D6D45C-954A-4270-8DD8-B4A135956956}" name="Description" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FCFCCF9B-859B-4CD1-ABB5-F858348FED0A}" name="Table15" displayName="Table15" ref="A24:F31" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FCFCCF9B-859B-4CD1-ABB5-F858348FED0A}" name="Table15" displayName="Table15" ref="A24:F31" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A24:F31" xr:uid="{52C67638-1B0C-4D81-A4CD-8C2F1FB32EE8}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{56A3FC9B-DA08-4FE7-8C24-8AC01910D63B}" name="Manufacturer" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{F1B37991-8950-4D23-A06D-551E68F8B3A7}" name="Part" dataDxfId="12" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{1D385C25-0E6D-4F87-970B-CD266BC98570}" name="Quantity" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{B8B8D3DC-E905-4196-A036-76A66D6CB7AF}" name="Unit Cost" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{C4CA4039-9456-447A-9CD1-BEEEEED1A36D}" name="Total Cost" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{56A3FC9B-DA08-4FE7-8C24-8AC01910D63B}" name="Manufacturer" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{F1B37991-8950-4D23-A06D-551E68F8B3A7}" name="Part" dataDxfId="15" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{1D385C25-0E6D-4F87-970B-CD266BC98570}" name="Quantity" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{B8B8D3DC-E905-4196-A036-76A66D6CB7AF}" name="Unit Cost" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{C4CA4039-9456-447A-9CD1-BEEEEED1A36D}" name="Total Cost" dataDxfId="12">
       <calculatedColumnFormula>C25*D25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4B415A4B-3C48-4690-B282-4B3F69FBFE3F}" name="Description" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{4B415A4B-3C48-4690-B282-4B3F69FBFE3F}" name="Description" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4F91D115-339B-49A3-AAEA-6EB7C7669611}" name="Table16" displayName="Table16" ref="A33:F38" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4F91D115-339B-49A3-AAEA-6EB7C7669611}" name="Table16" displayName="Table16" ref="A33:F38" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A33:F38" xr:uid="{DBEF985F-E018-4ABB-B45F-D1057C3E3471}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{54E445DD-98DA-46E3-A80B-8A50437F89C4}" name="Manufacturer" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{5FF8C2CC-5B67-4E6B-92F6-A699C3EA1584}" name="Part" dataDxfId="4" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{5C1A08AC-6112-4549-B5F6-6346E223FB0E}" name="Quantity" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{20BE8DBA-F191-4A95-ACB4-19DA62EF95E4}" name="Unit Cost" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{3E92051E-DDC0-4F11-9CEE-25F6B6A8FD76}" name="Total Cost" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{54E445DD-98DA-46E3-A80B-8A50437F89C4}" name="Manufacturer" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{5FF8C2CC-5B67-4E6B-92F6-A699C3EA1584}" name="Part" dataDxfId="7" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{5C1A08AC-6112-4549-B5F6-6346E223FB0E}" name="Quantity" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{20BE8DBA-F191-4A95-ACB4-19DA62EF95E4}" name="Unit Cost" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{3E92051E-DDC0-4F11-9CEE-25F6B6A8FD76}" name="Total Cost" dataDxfId="4">
       <calculatedColumnFormula>C34*D34</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{81E1B56B-A220-4D8E-82AD-13D4ED53E39E}" name="Description" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{81E1B56B-A220-4D8E-82AD-13D4ED53E39E}" name="Description" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B71291CB-1AB1-422A-91A8-5DED73C75C60}" name="Table1" displayName="Table1" ref="A40:F43" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A40:F43" xr:uid="{6DDA5838-F65B-47E2-80EF-DDB03E047663}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{4A09C7DE-FC3B-4D33-B44B-EA33206F6CB4}" name="Manufacturer"/>
+    <tableColumn id="2" xr3:uid="{51852398-FAB9-4CB3-B434-025665E3EAC4}" name="Part" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{8999A1DD-3C9C-4CFD-852B-28B03CD19A61}" name="Quantity"/>
+    <tableColumn id="4" xr3:uid="{C692534C-87E7-435B-A6D4-4AD47B9B4D1A}" name="Unit Cost" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{BDBEC533-3E47-4451-9550-FD4853A367CB}" name="Total Cost" dataDxfId="1">
+      <calculatedColumnFormula>C41*D41</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{0F39F248-3C38-4C64-88C7-2C0D6067B789}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -979,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF23C1D-2294-427C-B5AD-0FB9021529AC}">
-  <dimension ref="A2:F38"/>
+  <dimension ref="A2:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+      <selection activeCell="A40" sqref="A40:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -990,7 +1047,8 @@
     <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1796875" customWidth="1"/>
-    <col min="4" max="5" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" customWidth="1"/>
     <col min="6" max="6" width="104.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="103.36328125" customWidth="1"/>
   </cols>
@@ -1029,7 +1087,7 @@
         <v>2542</v>
       </c>
       <c r="E3" s="5">
-        <f>C3*D3</f>
+        <f t="shared" ref="E3:E14" si="0">C3*D3</f>
         <v>2542</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1050,7 +1108,7 @@
         <v>200</v>
       </c>
       <c r="E4" s="5">
-        <f>C4*D4</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -1071,7 +1129,7 @@
         <v>73</v>
       </c>
       <c r="E5" s="5">
-        <f>C5*D5</f>
+        <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -1092,7 +1150,7 @@
         <v>34</v>
       </c>
       <c r="E6" s="5">
-        <f>C6*D6</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1113,7 +1171,7 @@
         <v>22</v>
       </c>
       <c r="E7" s="5">
-        <f>C7*D7</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1134,7 +1192,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="5">
-        <f>C8*D8</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -1155,7 +1213,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="5">
-        <f>C9*D9</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -1176,7 +1234,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="5">
-        <f>C10*D10</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -1197,7 +1255,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="5">
-        <f>C11*D11</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -1218,7 +1276,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="5">
-        <f>C12*D12</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -1239,7 +1297,7 @@
         <v>6</v>
       </c>
       <c r="E13" s="5">
-        <f>C13*D13</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -1260,7 +1318,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="5">
-        <f>C14*D14</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -1636,6 +1694,89 @@
         <v>20</v>
       </c>
       <c r="F38" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" s="10">
+        <v>7</v>
+      </c>
+      <c r="E41" s="10">
+        <f>C41*D41</f>
+        <v>7</v>
+      </c>
+      <c r="F41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" s="10">
+        <v>7</v>
+      </c>
+      <c r="E42" s="10">
+        <f>C42*D42</f>
+        <v>7</v>
+      </c>
+      <c r="F42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" s="10">
+        <v>36</v>
+      </c>
+      <c r="E43" s="10">
+        <f>C43*D43</f>
+        <v>36</v>
+      </c>
+      <c r="F43" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1661,14 +1802,18 @@
     <hyperlink ref="B34" r:id="rId20" xr:uid="{9FDC3C94-EAF8-4C90-8489-20D443202A09}"/>
     <hyperlink ref="B35" r:id="rId21" xr:uid="{B9793429-3BDC-4184-BAD2-6165B67EC9AE}"/>
     <hyperlink ref="B36" r:id="rId22" xr:uid="{DFCA9B42-C6F3-4FA7-8E72-8961A8B57082}"/>
+    <hyperlink ref="B41" r:id="rId23" xr:uid="{AD84471F-E6C3-4328-BE1F-5BF62710799C}"/>
+    <hyperlink ref="B42" r:id="rId24" xr:uid="{2197AB9D-1F8D-4B35-AB97-FF8EF17713CB}"/>
+    <hyperlink ref="B43" r:id="rId25" xr:uid="{07A2CF34-51C0-4177-AF32-673BEB5AFA87}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId23"/>
-  <tableParts count="4">
-    <tablePart r:id="rId24"/>
-    <tablePart r:id="rId25"/>
-    <tablePart r:id="rId26"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId26"/>
+  <tableParts count="5">
     <tablePart r:id="rId27"/>
+    <tablePart r:id="rId28"/>
+    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId30"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>